<commit_message>
A new day has come
</commit_message>
<xml_diff>
--- a/Inter_blocking_probabilities.xlsx
+++ b/Inter_blocking_probabilities.xlsx
@@ -388,7 +388,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2258218895336587</v>
+        <v>2.517112612985156e-10</v>
       </c>
       <c r="C2" t="n">
         <v>2.293246651069942e-07</v>
@@ -402,7 +402,7 @@
         <v>1.5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2258790764600246</v>
+        <v>7.679762822577009e-09</v>
       </c>
       <c r="C3" t="n">
         <v>2.389469662438145e-06</v>
@@ -416,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2260203273039482</v>
+        <v>9.273040197581414e-08</v>
       </c>
       <c r="C4" t="n">
         <v>1.225308084902068e-05</v>
@@ -430,7 +430,7 @@
         <v>2.5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2262951106218263</v>
+        <v>6.725351380400409e-07</v>
       </c>
       <c r="C5" t="n">
         <v>4.256340808112286e-05</v>
@@ -444,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2267601366209196</v>
+        <v>3.521222073310612e-06</v>
       </c>
       <c r="C6" t="n">
         <v>0.0001154758122588428</v>
@@ -458,7 +458,7 @@
         <v>3.5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.22748031448616</v>
+        <v>1.467498748185719e-05</v>
       </c>
       <c r="C7" t="n">
         <v>0.0002639961999197263</v>
@@ -472,7 +472,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2285303958074612</v>
+        <v>5.161355800702858e-05</v>
       </c>
       <c r="C8" t="n">
         <v>0.0005321865558670192</v>
@@ -486,7 +486,7 @@
         <v>4.5</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2299960421193144</v>
+        <v>0.0001591403836677027</v>
       </c>
       <c r="C9" t="n">
         <v>0.0009741373237876633</v>
@@ -500,7 +500,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2319733600308843</v>
+        <v>0.0004416326008299711</v>
       </c>
       <c r="C10" t="n">
         <v>0.001651883461890281</v>
@@ -514,7 +514,7 @@
         <v>5.5</v>
       </c>
       <c r="B11" t="n">
-        <v>0.23456644977427</v>
+        <v>0.001124308218147197</v>
       </c>
       <c r="C11" t="n">
         <v>0.002632557747637834</v>

</xml_diff>

<commit_message>
Intra and Inter Slice Handover Implemented
</commit_message>
<xml_diff>
--- a/Inter_blocking_probabilities.xlsx
+++ b/Inter_blocking_probabilities.xlsx
@@ -1,37 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>eMBB</t>
+  </si>
+  <si>
+    <t>uRLLC</t>
+  </si>
+  <si>
+    <t>mMTC</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +63,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -353,177 +379,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>eMBB</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>uRLLC</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>mMTC</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>2.517112612985156e-10</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2.293246651069942e-07</v>
-      </c>
-      <c r="D2" t="n">
-        <v>6.172920928803185e-13</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3.687865850169651e-10</v>
+      </c>
+      <c r="C2">
+        <v>2.301951045209976e-07</v>
+      </c>
+      <c r="D2">
+        <v>1.432909306761138e-12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
         <v>1.5</v>
       </c>
-      <c r="B3" t="n">
-        <v>7.679762822577009e-09</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2.389469662438145e-06</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4.650254770553579e-11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="B3">
+        <v>1.74963016796531</v>
+      </c>
+      <c r="C3">
+        <v>0.1016721856136527</v>
+      </c>
+      <c r="D3">
+        <v>0.3068015775388266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>9.273040197581414e-08</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.225308084902068e-05</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.086034173961883e-09</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="B4">
+        <v>2281.331904622818</v>
+      </c>
+      <c r="C4">
+        <v>0.6116070947018161</v>
+      </c>
+      <c r="D4">
+        <v>47.56962772687632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>2.5</v>
       </c>
-      <c r="B5" t="n">
-        <v>6.725351380400409e-07</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4.256340808112286e-05</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.33870102710534e-08</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="B5">
+        <v>178125.9621508546</v>
+      </c>
+      <c r="C5">
+        <v>0.8695877792903342</v>
+      </c>
+      <c r="D5">
+        <v>701.487278961415</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" t="n">
-        <v>3.521222073310612e-06</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.0001154758122588428</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.103402513445827e-07</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="B6">
+        <v>3492479.918757605</v>
+      </c>
+      <c r="C6">
+        <v>0.9499230125033209</v>
+      </c>
+      <c r="D6">
+        <v>4379.42362620887</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
         <v>3.5</v>
       </c>
-      <c r="B7" t="n">
-        <v>1.467498748185719e-05</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0002639961999197263</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6.894144124266861e-07</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="B7">
+        <v>33072280.0301702</v>
+      </c>
+      <c r="C7">
+        <v>0.9775415798139849</v>
+      </c>
+      <c r="D7">
+        <v>18234.99529533953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" t="n">
-        <v>5.161355800702858e-05</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0005321865558670192</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3.515121335090763e-06</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="B8">
+        <v>203085323.1611342</v>
+      </c>
+      <c r="C8">
+        <v>0.988612893062402</v>
+      </c>
+      <c r="D8">
+        <v>59308.27040661886</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
         <v>4.5</v>
       </c>
-      <c r="B9" t="n">
-        <v>0.0001591403836677027</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.0009741373237876633</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.530982676993621e-05</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="B9">
+        <v>934680959.0368755</v>
+      </c>
+      <c r="C9">
+        <v>0.9936605142969975</v>
+      </c>
+      <c r="D9">
+        <v>162536.4095940694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
         <v>5</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.0004416326008299711</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.001651883461890281</v>
-      </c>
-      <c r="D10" t="n">
-        <v>5.860212509809892e-05</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="B10">
+        <v>3497048501.822735</v>
+      </c>
+      <c r="C10">
+        <v>0.9962064790987923</v>
+      </c>
+      <c r="D10">
+        <v>392287.5500086435</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
         <v>5.5</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.001124308218147197</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.002632557747637834</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0002003676996185919</v>
+      <c r="B11">
+        <v>11187302191.36667</v>
+      </c>
+      <c r="C11">
+        <v>0.9975969773766412</v>
+      </c>
+      <c r="D11">
+        <v>858075.4030528213</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>